<commit_message>
New user added to NUsers.xlsx
</commit_message>
<xml_diff>
--- a/NUsers.xlsx
+++ b/NUsers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -104,13 +104,37 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>mohanl@gmai.com</t>
+  </si>
+  <si>
+    <t>MohanLal@123</t>
+  </si>
+  <si>
+    <t>Com34</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -120,6 +144,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -148,6 +177,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,6 +511,44 @@
         <v>9.087614512E9</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="4">
+        <v>700987.0</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="4">
+        <v>9.785613012E9</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>